<commit_message>
Added blinky, updated bring-up doc and added fixes doc
</commit_message>
<xml_diff>
--- a/Documentation/Bring-Up Testing Overview.xlsx
+++ b/Documentation/Bring-Up Testing Overview.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\msx\bs\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{430BF95C-2A94-4267-8AF4-D9A5F1EC1962}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9ECD1CD-0079-433F-8F0C-702403446A99}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="23640" tabRatio="766" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="766" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="6" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="88">
   <si>
     <t>(-) Terminal</t>
   </si>
@@ -229,24 +229,9 @@
     <t>Load test firmware via Arduino IDE, verify LEDs flash</t>
   </si>
   <si>
-    <t>Load test firmware using programmer and Tag Connect, verify LEDs flash</t>
-  </si>
-  <si>
-    <t>USB TTL Bridge + Autoreset</t>
-  </si>
-  <si>
-    <t>Load test BLE firmware and verify connection with phone</t>
-  </si>
-  <si>
     <t>DFU Header</t>
   </si>
   <si>
-    <t>Button Press + User LEDs</t>
-  </si>
-  <si>
-    <t>Use test firmware to confirm button press turns on user LED, other LED runs as heartbeat</t>
-  </si>
-  <si>
     <t>LDO Input Selection</t>
   </si>
   <si>
@@ -277,12 +262,6 @@
     <t>Remove R3, Replace R4 = 47ohm, Cut SW1.3-4, Wire SW1.3 to SW1.6</t>
   </si>
   <si>
-    <t>Remove D4, Q1 and short DS</t>
-  </si>
-  <si>
-    <t>Replace in next version (see above)</t>
-  </si>
-  <si>
     <t>Knocked D1 off</t>
   </si>
   <si>
@@ -305,13 +284,31 @@
   </si>
   <si>
     <t>Lot of flux left over, bad silk, components weak/lifted; D1/D7 fell off</t>
+  </si>
+  <si>
+    <t>Load new bootloader using programmer and Tag Connect, verify OK</t>
+  </si>
+  <si>
+    <t>https://bit.ly/2woV9Cv</t>
+  </si>
+  <si>
+    <t>USB TTL Bridge + Autoreset + User LEDs</t>
+  </si>
+  <si>
+    <t>Load sample beacon or controller BLE firmware and verify connection with phone</t>
+  </si>
+  <si>
+    <t>Removed D4, Q1 and short DS</t>
+  </si>
+  <si>
+    <t>Removed on board 1/2 (see above); worked on board 3 when reseated</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -331,6 +328,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -416,10 +421,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -456,7 +462,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
@@ -481,6 +486,10 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -491,7 +500,8 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -770,29 +780,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:L21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="85.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="9.140625" customWidth="1"/>
-    <col min="5" max="5" width="63.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="35.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="9.109375" customWidth="1"/>
+    <col min="5" max="5" width="63.44140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
-        <v>71</v>
-      </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
+    <row r="1" spans="1:12" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="32" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="32"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
       <c r="F1" s="8"/>
       <c r="G1" s="8"/>
       <c r="H1" s="8"/>
@@ -801,17 +811,17 @@
       <c r="K1" s="8"/>
       <c r="L1" s="8"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="32"/>
+      <c r="D2" s="33"/>
       <c r="E2" s="9" t="s">
         <v>9</v>
       </c>
@@ -823,7 +833,7 @@
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="10"/>
       <c r="B3" s="10"/>
       <c r="C3" s="2">
@@ -834,26 +844,26 @@
       </c>
       <c r="E3" s="10"/>
       <c r="F3" s="3"/>
-      <c r="G3" s="33" t="s">
+      <c r="G3" s="34" t="s">
         <v>10</v>
       </c>
-      <c r="H3" s="33"/>
+      <c r="H3" s="34"/>
       <c r="I3" s="3"/>
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>11</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="30"/>
+      <c r="C4" s="29"/>
+      <c r="D4" s="29"/>
       <c r="E4" s="3" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="13"/>
@@ -865,7 +875,7 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>27</v>
       </c>
@@ -880,7 +890,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
         <v>17</v>
       </c>
@@ -895,7 +905,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
         <v>19</v>
       </c>
@@ -910,7 +920,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
         <v>20</v>
       </c>
@@ -921,129 +931,124 @@
       <c r="D8" s="11"/>
       <c r="E8" s="3"/>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="B9" s="12" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D9" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E9" s="18" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C9" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D9" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B10" s="27" t="s">
+      <c r="B10" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="C10" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="D10" s="29" t="s">
-        <v>77</v>
-      </c>
-      <c r="E10" s="18" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C10" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B11" s="27" t="s">
+      <c r="B11" s="26" t="s">
         <v>60</v>
       </c>
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
       <c r="E11" s="3"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B12" s="27" t="s">
-        <v>70</v>
-      </c>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
+        <v>64</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>65</v>
+      </c>
+      <c r="C12" s="28" t="s">
+        <v>72</v>
+      </c>
+      <c r="D12" s="28" t="s">
+        <v>72</v>
+      </c>
       <c r="E12" s="3" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B13" s="27" t="s">
-        <v>63</v>
-      </c>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B13" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="C13" s="31"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="30" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B14" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="B14" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="11"/>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B15" s="27" t="s">
-        <v>68</v>
+        <v>23</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>85</v>
       </c>
       <c r="C15" s="12"/>
       <c r="D15" s="12"/>
       <c r="E15" s="3"/>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16" s="27" t="s">
-        <v>65</v>
+        <v>63</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>25</v>
       </c>
       <c r="C16" s="12"/>
       <c r="D16" s="12"/>
       <c r="E16" s="3"/>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="23" t="s">
-        <v>25</v>
-      </c>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C17" s="12"/>
       <c r="D17" s="12"/>
-      <c r="E17" s="3"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
       <c r="C18" s="12"/>
       <c r="D18" s="12"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="C19" s="12"/>
-      <c r="D19" s="12"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="B21" t="s">
         <v>26</v>
       </c>
     </row>
@@ -1053,6 +1058,9 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="G3:H3"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="E13" r:id="rId1" xr:uid="{34160FE2-1DAC-4E10-A118-158343E04501}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>
 </worksheet>
@@ -1066,27 +1074,27 @@
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" customWidth="1"/>
-    <col min="3" max="4" width="7.140625" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="4" width="7.109375" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="32"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="D1" s="33"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
       <c r="B2" s="10"/>
       <c r="C2" s="2">
@@ -1096,20 +1104,20 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>30</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C3" s="28"/>
-      <c r="D3" s="28"/>
+      <c r="C3" s="27"/>
+      <c r="D3" s="27"/>
       <c r="E3" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1119,7 +1127,7 @@
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>32</v>
       </c>
@@ -1129,7 +1137,7 @@
       <c r="C5" s="11"/>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>33</v>
       </c>
@@ -1139,7 +1147,7 @@
       <c r="C6" s="11"/>
       <c r="D6" s="11"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>34</v>
       </c>
@@ -1149,7 +1157,7 @@
       <c r="C7" s="11"/>
       <c r="D7" s="11"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>35</v>
       </c>
@@ -1159,17 +1167,17 @@
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
         <v>37</v>
       </c>
@@ -1179,7 +1187,7 @@
       <c r="C10" s="11"/>
       <c r="D10" s="11"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
         <v>38</v>
       </c>
@@ -1189,11 +1197,11 @@
       <c r="C11" s="11"/>
       <c r="D11" s="11"/>
     </row>
-    <row r="25" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
     </row>
-    <row r="28" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="3:4" x14ac:dyDescent="0.3">
       <c r="C28" s="7"/>
       <c r="D28" s="7"/>
     </row>
@@ -1214,28 +1222,28 @@
       <selection activeCell="H9" sqref="F3:H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="13.28515625" customWidth="1"/>
+    <col min="1" max="1" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="33" t="s">
         <v>24</v>
       </c>
-      <c r="D1" s="32"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D1" s="33"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="10"/>
-      <c r="B2" s="20"/>
+      <c r="B2" s="19"/>
       <c r="C2" s="2">
         <v>1</v>
       </c>
@@ -1243,65 +1251,65 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>52</v>
       </c>
-      <c r="C3" s="19"/>
+      <c r="C3" s="18"/>
       <c r="D3" s="11"/>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="19"/>
+      <c r="C4" s="18"/>
       <c r="D4" s="11"/>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>44</v>
       </c>
       <c r="B5" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="19"/>
+      <c r="C5" s="18"/>
       <c r="D5" s="11"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>47</v>
       </c>
       <c r="B6" t="s">
         <v>51</v>
       </c>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="19"/>
-      <c r="D7" s="19"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>48</v>
       </c>
       <c r="B8" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1320,93 +1328,93 @@
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="B1" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="C1" s="22" t="s">
+      <c r="C1" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="D1" s="22" t="s">
+      <c r="D1" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E1" s="22" t="s">
+      <c r="E1" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="F1" s="22" t="s">
+      <c r="F1" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="22" t="s">
+      <c r="G1" s="21" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" s="24" t="s">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
         <v>45</v>
       </c>
       <c r="B2" s="4"/>
       <c r="C2" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="23" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="23" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="G4" s="25" t="s">
-        <v>82</v>
-      </c>
-      <c r="H4" s="25" t="s">
+      <c r="E4" s="25" t="s">
+        <v>75</v>
+      </c>
+      <c r="F4" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="G4" s="24" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="24" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="23" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="4"/>
@@ -1414,14 +1422,14 @@
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="3" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="23" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="4"/>
@@ -1430,11 +1438,11 @@
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="G6" s="3" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="23" t="s">
         <v>48</v>
       </c>
       <c r="B7" s="4"/>
@@ -1444,7 +1452,7 @@
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I13" s="15" t="s">
         <v>45</v>
       </c>
@@ -1452,7 +1460,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I14" s="15" t="s">
         <v>46</v>
       </c>
@@ -1460,7 +1468,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I15" s="15" t="s">
         <v>44</v>
       </c>
@@ -1468,7 +1476,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="I16" s="15" t="s">
         <v>47</v>
       </c>
@@ -1476,7 +1484,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="17" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I17" s="15" t="s">
         <v>2</v>
       </c>
@@ -1484,7 +1492,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="9:10" x14ac:dyDescent="0.25">
+    <row r="18" spans="9:10" x14ac:dyDescent="0.3">
       <c r="I18" s="15" t="s">
         <v>48</v>
       </c>
@@ -1506,26 +1514,26 @@
       <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="D1" s="32"/>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="20"/>
+      <c r="D1" s="33"/>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2" s="20"/>
+      <c r="B2" s="19"/>
       <c r="C2" s="2">
         <v>1</v>
       </c>
@@ -1533,7 +1541,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>45</v>
       </c>
@@ -1541,27 +1549,27 @@
         <v>52</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="19" t="s">
-        <v>75</v>
+      <c r="C4" s="18" t="s">
+        <v>70</v>
       </c>
       <c r="D4" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>44</v>
       </c>
@@ -1569,13 +1577,13 @@
         <v>50</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>47</v>
       </c>
@@ -1583,38 +1591,38 @@
         <v>51</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>2</v>
       </c>
       <c r="B7" t="s">
         <v>49</v>
       </c>
-      <c r="C7" s="19" t="s">
-        <v>75</v>
+      <c r="C7" s="18" t="s">
+        <v>70</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>48</v>
       </c>
       <c r="B8" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="19" t="s">
+      <c r="C8" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="18" t="s">
         <v>76</v>
-      </c>
-      <c r="D8" s="19" t="s">
-        <v>83</v>
       </c>
     </row>
   </sheetData>

</xml_diff>